<commit_message>
invoice data and blank invoice template
</commit_message>
<xml_diff>
--- a/src/python/comp-230/invoice_blank.xlsx
+++ b/src/python/comp-230/invoice_blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dalton/Code/cohort3/src/python/comp-230/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7351BC-CDF6-5D4F-975E-18653802DB14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5796AE-78A0-344A-83F6-795C18895495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="22020" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>[Company Name]</t>
   </si>
@@ -54,9 +54,6 @@
     <t>https://www.vertex42.com/ExcelTemplates/invoice-templates.html</t>
   </si>
   <si>
-    <t>Phone: (000) 000-0000</t>
-  </si>
-  <si>
     <t>INVOICE #</t>
   </si>
   <si>
@@ -163,6 +160,12 @@
   </si>
   <si>
     <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone: </t>
+  </si>
+  <si>
+    <t>1-234-567-8901</t>
   </si>
 </sst>
 </file>
@@ -1634,8 +1637,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1693,18 +1696,20 @@
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
       <c r="F4" s="58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="58"/>
       <c r="H4" s="52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J4" s="32"/>
     </row>
@@ -1736,26 +1741,26 @@
     </row>
     <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="61"/>
       <c r="C7" s="61"/>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="58"/>
       <c r="H7" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="32" t="s">
         <v>11</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1766,7 +1771,7 @@
       </c>
       <c r="G8" s="60"/>
       <c r="H8" s="53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="32"/>
     </row>
@@ -1808,12 +1813,12 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="J11" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1823,12 +1828,12 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="J12" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1838,7 +1843,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="J13" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1851,31 +1856,31 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="J14" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="54"/>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="52" t="s">
+      <c r="H15" s="52" t="s">
         <v>23</v>
-      </c>
-      <c r="H15" s="52" t="s">
-        <v>24</v>
       </c>
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -1895,7 +1900,7 @@
     </row>
     <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -1915,7 +1920,7 @@
     </row>
     <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -1930,7 +1935,7 @@
         <v>-50</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2103,14 +2108,14 @@
     </row>
     <row r="31" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="62"/>
       <c r="C31" s="62"/>
       <c r="D31" s="62"/>
       <c r="E31" s="62"/>
       <c r="F31" s="63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G31" s="63"/>
       <c r="H31" s="28">
@@ -2126,14 +2131,14 @@
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G32" s="63"/>
       <c r="H32" s="29">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2143,7 +2148,7 @@
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
       <c r="F33" s="55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" s="55"/>
       <c r="H33" s="28">
@@ -2159,7 +2164,7 @@
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G34" s="64"/>
       <c r="H34" s="19">
@@ -2167,7 +2172,7 @@
         <v>547.3125</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -2180,7 +2185,7 @@
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
       <c r="J35" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2196,7 +2201,7 @@
     </row>
     <row r="37" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="65"/>
       <c r="C37" s="65"/>
@@ -2209,7 +2214,7 @@
     </row>
     <row r="38" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="57"/>
       <c r="C38" s="57"/>
@@ -2219,7 +2224,7 @@
       <c r="G38" s="57"/>
       <c r="H38" s="57"/>
       <c r="J38" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2287,12 +2292,12 @@
     <row r="4" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:2" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
@@ -2300,7 +2305,7 @@
     </row>
     <row r="8" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>